<commit_message>
them app nhap du lieu va file thong ke giao dich
</commit_message>
<xml_diff>
--- a/2023/DongTien.xlsx
+++ b/2023/DongTien.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trung.nguyenhoang/Documents/github/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C0ACCF-883B-434D-8335-B94E6867216B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3BEB7F-4DD4-5746-9B66-FDF1EB5B4DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17080" xr2:uid="{42582BF8-9AD7-9540-81DE-245C476BF20D}"/>
   </bookViews>
@@ -560,28 +560,25 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -596,27 +593,28 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC78DB7-94EE-DD4A-955E-8CCDACC517C9}">
   <dimension ref="A1:GP40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="CA1" workbookViewId="0">
+      <selection activeCell="CL1" sqref="CL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -985,465 +983,465 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:198" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="38" t="s">
+      <c r="S1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="38"/>
-      <c r="AC1" s="38"/>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="38"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="38"/>
-      <c r="AJ1" s="38"/>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="38"/>
-      <c r="AM1" s="38"/>
-      <c r="AN1" s="38"/>
-      <c r="AO1" s="38"/>
-      <c r="AP1" s="38"/>
-      <c r="AQ1" s="38"/>
-      <c r="AR1" s="38"/>
-      <c r="AS1" s="39" t="s">
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="41"/>
+      <c r="AE1" s="41"/>
+      <c r="AF1" s="41"/>
+      <c r="AG1" s="41"/>
+      <c r="AH1" s="41"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="41"/>
+      <c r="AK1" s="41"/>
+      <c r="AL1" s="41"/>
+      <c r="AM1" s="41"/>
+      <c r="AN1" s="41"/>
+      <c r="AO1" s="41"/>
+      <c r="AP1" s="41"/>
+      <c r="AQ1" s="41"/>
+      <c r="AR1" s="41"/>
+      <c r="AS1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="AT1" s="39"/>
-      <c r="AU1" s="39"/>
-      <c r="AV1" s="39"/>
-      <c r="AW1" s="39"/>
-      <c r="AX1" s="39"/>
-      <c r="AY1" s="39"/>
-      <c r="AZ1" s="39"/>
-      <c r="BA1" s="39"/>
-      <c r="BB1" s="39"/>
-      <c r="BC1" s="39"/>
-      <c r="BD1" s="39"/>
-      <c r="BE1" s="39"/>
-      <c r="BF1" s="39"/>
-      <c r="BG1" s="39"/>
-      <c r="BH1" s="39"/>
-      <c r="BI1" s="39"/>
+      <c r="AT1" s="51"/>
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="51"/>
+      <c r="AW1" s="51"/>
+      <c r="AX1" s="51"/>
+      <c r="AY1" s="51"/>
+      <c r="AZ1" s="51"/>
+      <c r="BA1" s="51"/>
+      <c r="BB1" s="51"/>
+      <c r="BC1" s="51"/>
+      <c r="BD1" s="51"/>
+      <c r="BE1" s="51"/>
+      <c r="BF1" s="51"/>
+      <c r="BG1" s="51"/>
+      <c r="BH1" s="51"/>
+      <c r="BI1" s="51"/>
       <c r="BJ1" s="1"/>
-      <c r="BK1" s="48"/>
-      <c r="BL1" s="48"/>
-      <c r="BM1" s="48"/>
-      <c r="BN1" s="48"/>
-      <c r="BO1" s="48"/>
-      <c r="BP1" s="48"/>
-      <c r="BQ1" s="48"/>
-      <c r="BR1" s="48"/>
-      <c r="BS1" s="48"/>
-      <c r="BT1" s="48"/>
-      <c r="BU1" s="48"/>
-      <c r="BV1" s="48"/>
-      <c r="BW1" s="48"/>
-      <c r="BX1" s="48"/>
-      <c r="BY1" s="48"/>
-      <c r="BZ1" s="48"/>
-      <c r="CA1" s="48"/>
-      <c r="CB1" s="48"/>
-      <c r="CC1" s="48"/>
-      <c r="CD1" s="48"/>
-      <c r="CE1" s="48"/>
-      <c r="CF1" s="48"/>
-      <c r="CG1" s="48"/>
-      <c r="CH1" s="48"/>
-      <c r="CI1" s="48"/>
-      <c r="CJ1" s="48"/>
-      <c r="CK1" s="48"/>
-      <c r="CL1" s="49" t="s">
+      <c r="BK1" s="40"/>
+      <c r="BL1" s="40"/>
+      <c r="BM1" s="40"/>
+      <c r="BN1" s="40"/>
+      <c r="BO1" s="40"/>
+      <c r="BP1" s="40"/>
+      <c r="BQ1" s="40"/>
+      <c r="BR1" s="40"/>
+      <c r="BS1" s="40"/>
+      <c r="BT1" s="40"/>
+      <c r="BU1" s="40"/>
+      <c r="BV1" s="40"/>
+      <c r="BW1" s="40"/>
+      <c r="BX1" s="40"/>
+      <c r="BY1" s="40"/>
+      <c r="BZ1" s="40"/>
+      <c r="CA1" s="40"/>
+      <c r="CB1" s="40"/>
+      <c r="CC1" s="40"/>
+      <c r="CD1" s="40"/>
+      <c r="CE1" s="40"/>
+      <c r="CF1" s="40"/>
+      <c r="CG1" s="40"/>
+      <c r="CH1" s="40"/>
+      <c r="CI1" s="40"/>
+      <c r="CJ1" s="40"/>
+      <c r="CK1" s="40"/>
+      <c r="CL1" s="1"/>
+      <c r="CM1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="CM1" s="49"/>
-      <c r="CN1" s="49"/>
-      <c r="CO1" s="49"/>
-      <c r="CP1" s="49"/>
-      <c r="CQ1" s="49"/>
-      <c r="CR1" s="49"/>
-      <c r="CS1" s="49"/>
-      <c r="CT1" s="49"/>
-      <c r="CU1" s="49"/>
-      <c r="CV1" s="49"/>
-      <c r="CW1" s="49"/>
-      <c r="CX1" s="49"/>
-      <c r="CY1" s="49"/>
-      <c r="CZ1" s="49"/>
-      <c r="DA1" s="49"/>
-      <c r="DB1" s="49"/>
-      <c r="DC1" s="49"/>
-      <c r="DD1" s="49"/>
-      <c r="DE1" s="49"/>
-      <c r="DF1" s="49"/>
-      <c r="DG1" s="49"/>
-      <c r="DH1" s="49"/>
-      <c r="DI1" s="49"/>
-      <c r="DJ1" s="49"/>
-      <c r="DK1" s="49"/>
-      <c r="DL1" s="49"/>
-      <c r="DM1" s="49"/>
-      <c r="DN1" s="49"/>
-      <c r="DO1" s="49"/>
-      <c r="DP1" s="49"/>
-      <c r="DQ1" s="49"/>
-      <c r="DR1" s="49"/>
-      <c r="DS1" s="49"/>
-      <c r="DT1" s="49"/>
-      <c r="DU1" s="49"/>
-      <c r="DV1" s="49"/>
-      <c r="DW1" s="49"/>
-      <c r="DX1" s="49"/>
-      <c r="DY1" s="49"/>
-      <c r="DZ1" s="49"/>
-      <c r="EA1" s="49"/>
-      <c r="EB1" s="49"/>
-      <c r="EC1" s="49"/>
-      <c r="ED1" s="1"/>
-      <c r="EE1" s="44" t="s">
+      <c r="CN1" s="56"/>
+      <c r="CO1" s="56"/>
+      <c r="CP1" s="56"/>
+      <c r="CQ1" s="56"/>
+      <c r="CR1" s="56"/>
+      <c r="CS1" s="56"/>
+      <c r="CT1" s="56"/>
+      <c r="CU1" s="56"/>
+      <c r="CV1" s="56"/>
+      <c r="CW1" s="56"/>
+      <c r="CX1" s="56"/>
+      <c r="CY1" s="56"/>
+      <c r="CZ1" s="56"/>
+      <c r="DA1" s="56"/>
+      <c r="DB1" s="56"/>
+      <c r="DC1" s="56"/>
+      <c r="DD1" s="56"/>
+      <c r="DE1" s="56"/>
+      <c r="DF1" s="56"/>
+      <c r="DG1" s="56"/>
+      <c r="DH1" s="56"/>
+      <c r="DI1" s="56"/>
+      <c r="DJ1" s="56"/>
+      <c r="DK1" s="56"/>
+      <c r="DL1" s="56"/>
+      <c r="DM1" s="56"/>
+      <c r="DN1" s="56"/>
+      <c r="DO1" s="56"/>
+      <c r="DP1" s="56"/>
+      <c r="DQ1" s="56"/>
+      <c r="DR1" s="56"/>
+      <c r="DS1" s="56"/>
+      <c r="DT1" s="56"/>
+      <c r="DU1" s="56"/>
+      <c r="DV1" s="56"/>
+      <c r="DW1" s="56"/>
+      <c r="DX1" s="56"/>
+      <c r="DY1" s="56"/>
+      <c r="DZ1" s="56"/>
+      <c r="EA1" s="56"/>
+      <c r="EB1" s="56"/>
+      <c r="EC1" s="56"/>
+      <c r="ED1" s="56"/>
+      <c r="EE1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="EF1" s="44"/>
-      <c r="EG1" s="44"/>
-      <c r="EH1" s="44"/>
-      <c r="EI1" s="44"/>
-      <c r="EJ1" s="44"/>
-      <c r="EK1" s="44"/>
-      <c r="EL1" s="44"/>
-      <c r="EM1" s="44"/>
-      <c r="EN1" s="44"/>
-      <c r="EO1" s="44"/>
-      <c r="EP1" s="44"/>
-      <c r="EQ1" s="44"/>
-      <c r="ER1" s="44"/>
-      <c r="ES1" s="44"/>
-      <c r="ET1" s="44"/>
-      <c r="EU1" s="44"/>
+      <c r="EF1" s="45"/>
+      <c r="EG1" s="45"/>
+      <c r="EH1" s="45"/>
+      <c r="EI1" s="45"/>
+      <c r="EJ1" s="45"/>
+      <c r="EK1" s="45"/>
+      <c r="EL1" s="45"/>
+      <c r="EM1" s="45"/>
+      <c r="EN1" s="45"/>
+      <c r="EO1" s="45"/>
+      <c r="EP1" s="45"/>
+      <c r="EQ1" s="45"/>
+      <c r="ER1" s="45"/>
+      <c r="ES1" s="45"/>
+      <c r="ET1" s="45"/>
+      <c r="EU1" s="45"/>
       <c r="EV1" s="1"/>
-      <c r="EW1" s="50" t="s">
+      <c r="EW1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="EX1" s="50"/>
-      <c r="EY1" s="50"/>
-      <c r="EZ1" s="50"/>
-      <c r="FA1" s="50"/>
-      <c r="FB1" s="50"/>
-      <c r="FC1" s="50"/>
-      <c r="FD1" s="50"/>
-      <c r="FE1" s="50"/>
-      <c r="FF1" s="50"/>
-      <c r="FG1" s="50"/>
-      <c r="FH1" s="50"/>
-      <c r="FI1" s="50"/>
-      <c r="FJ1" s="50"/>
-      <c r="FK1" s="50"/>
-      <c r="FL1" s="50"/>
-      <c r="FM1" s="50"/>
-      <c r="FN1" s="50"/>
+      <c r="EX1" s="49"/>
+      <c r="EY1" s="49"/>
+      <c r="EZ1" s="49"/>
+      <c r="FA1" s="49"/>
+      <c r="FB1" s="49"/>
+      <c r="FC1" s="49"/>
+      <c r="FD1" s="49"/>
+      <c r="FE1" s="49"/>
+      <c r="FF1" s="49"/>
+      <c r="FG1" s="49"/>
+      <c r="FH1" s="49"/>
+      <c r="FI1" s="49"/>
+      <c r="FJ1" s="49"/>
+      <c r="FK1" s="49"/>
+      <c r="FL1" s="49"/>
+      <c r="FM1" s="49"/>
+      <c r="FN1" s="49"/>
       <c r="FO1" s="1"/>
-      <c r="FP1" s="47" t="s">
+      <c r="FP1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="FQ1" s="47"/>
-      <c r="FR1" s="47"/>
-      <c r="FS1" s="47"/>
-      <c r="FT1" s="47"/>
-      <c r="FU1" s="47"/>
-      <c r="FV1" s="47"/>
-      <c r="FW1" s="47"/>
+      <c r="FQ1" s="48"/>
+      <c r="FR1" s="48"/>
+      <c r="FS1" s="48"/>
+      <c r="FT1" s="48"/>
+      <c r="FU1" s="48"/>
+      <c r="FV1" s="48"/>
+      <c r="FW1" s="48"/>
       <c r="FX1" s="1"/>
-      <c r="FY1" s="46" t="s">
+      <c r="FY1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="FZ1" s="46"/>
-      <c r="GA1" s="46"/>
-      <c r="GB1" s="46"/>
-      <c r="GC1" s="46"/>
-      <c r="GD1" s="46"/>
-      <c r="GE1" s="46"/>
-      <c r="GF1" s="46"/>
+      <c r="FZ1" s="47"/>
+      <c r="GA1" s="47"/>
+      <c r="GB1" s="47"/>
+      <c r="GC1" s="47"/>
+      <c r="GD1" s="47"/>
+      <c r="GE1" s="47"/>
+      <c r="GF1" s="47"/>
       <c r="GG1" s="1"/>
-      <c r="GH1" s="45" t="s">
+      <c r="GH1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="GI1" s="45"/>
-      <c r="GJ1" s="45"/>
-      <c r="GK1" s="45"/>
-      <c r="GL1" s="45"/>
-      <c r="GM1" s="45"/>
-      <c r="GN1" s="45"/>
-      <c r="GO1" s="45"/>
+      <c r="GI1" s="46"/>
+      <c r="GJ1" s="46"/>
+      <c r="GK1" s="46"/>
+      <c r="GL1" s="46"/>
+      <c r="GM1" s="46"/>
+      <c r="GN1" s="46"/>
+      <c r="GO1" s="46"/>
       <c r="GP1" s="1"/>
     </row>
     <row r="2" spans="1:198" x14ac:dyDescent="0.2">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
       <c r="R2" s="1"/>
-      <c r="S2" s="40" t="s">
+      <c r="S2" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="44"/>
       <c r="AA2" s="1"/>
-      <c r="AB2" s="40" t="s">
+      <c r="AB2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="40"/>
-      <c r="AF2" s="40"/>
-      <c r="AG2" s="40"/>
-      <c r="AH2" s="40"/>
-      <c r="AI2" s="40"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
+      <c r="AF2" s="44"/>
+      <c r="AG2" s="44"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
       <c r="AJ2" s="1"/>
-      <c r="AK2" s="40" t="s">
+      <c r="AK2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="AL2" s="40"/>
-      <c r="AM2" s="40"/>
-      <c r="AN2" s="40"/>
-      <c r="AO2" s="40"/>
-      <c r="AP2" s="40"/>
-      <c r="AQ2" s="40"/>
-      <c r="AR2" s="40"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
       <c r="AS2" s="1"/>
-      <c r="AT2" s="40" t="s">
+      <c r="AT2" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="AU2" s="40"/>
-      <c r="AV2" s="40"/>
-      <c r="AW2" s="40"/>
-      <c r="AX2" s="40"/>
-      <c r="AY2" s="40"/>
-      <c r="AZ2" s="40"/>
-      <c r="BA2" s="40"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
+      <c r="AW2" s="44"/>
+      <c r="AX2" s="44"/>
+      <c r="AY2" s="44"/>
+      <c r="AZ2" s="44"/>
+      <c r="BA2" s="44"/>
       <c r="BB2" s="1"/>
-      <c r="BC2" s="41" t="s">
+      <c r="BC2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="BD2" s="42"/>
-      <c r="BE2" s="42"/>
-      <c r="BF2" s="42"/>
-      <c r="BG2" s="42"/>
-      <c r="BH2" s="42"/>
-      <c r="BI2" s="42"/>
-      <c r="BJ2" s="43"/>
+      <c r="BD2" s="53"/>
+      <c r="BE2" s="53"/>
+      <c r="BF2" s="53"/>
+      <c r="BG2" s="53"/>
+      <c r="BH2" s="53"/>
+      <c r="BI2" s="53"/>
+      <c r="BJ2" s="54"/>
       <c r="BK2" s="1"/>
-      <c r="BL2" s="41" t="s">
+      <c r="BL2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="BM2" s="42"/>
-      <c r="BN2" s="42"/>
-      <c r="BO2" s="42"/>
-      <c r="BP2" s="42"/>
-      <c r="BQ2" s="42"/>
-      <c r="BR2" s="43"/>
+      <c r="BM2" s="53"/>
+      <c r="BN2" s="53"/>
+      <c r="BO2" s="53"/>
+      <c r="BP2" s="53"/>
+      <c r="BQ2" s="53"/>
+      <c r="BR2" s="54"/>
       <c r="BS2" s="2"/>
       <c r="BT2" s="1"/>
-      <c r="BU2" s="40" t="s">
+      <c r="BU2" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="BV2" s="40"/>
-      <c r="BW2" s="40"/>
-      <c r="BX2" s="40"/>
-      <c r="BY2" s="40"/>
-      <c r="BZ2" s="40"/>
-      <c r="CA2" s="40"/>
-      <c r="CB2" s="40"/>
+      <c r="BV2" s="44"/>
+      <c r="BW2" s="44"/>
+      <c r="BX2" s="44"/>
+      <c r="BY2" s="44"/>
+      <c r="BZ2" s="44"/>
+      <c r="CA2" s="44"/>
+      <c r="CB2" s="44"/>
       <c r="CC2" s="1"/>
-      <c r="CD2" s="40" t="s">
+      <c r="CD2" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="CE2" s="40"/>
-      <c r="CF2" s="40"/>
-      <c r="CG2" s="40"/>
-      <c r="CH2" s="40"/>
-      <c r="CI2" s="40"/>
-      <c r="CJ2" s="40"/>
-      <c r="CK2" s="40"/>
+      <c r="CE2" s="44"/>
+      <c r="CF2" s="44"/>
+      <c r="CG2" s="44"/>
+      <c r="CH2" s="44"/>
+      <c r="CI2" s="44"/>
+      <c r="CJ2" s="44"/>
+      <c r="CK2" s="44"/>
       <c r="CL2" s="1"/>
-      <c r="CM2" s="40" t="s">
+      <c r="CM2" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="CN2" s="40"/>
-      <c r="CO2" s="40"/>
-      <c r="CP2" s="40"/>
-      <c r="CQ2" s="40"/>
-      <c r="CR2" s="40"/>
-      <c r="CS2" s="40"/>
-      <c r="CT2" s="40"/>
+      <c r="CN2" s="44"/>
+      <c r="CO2" s="44"/>
+      <c r="CP2" s="44"/>
+      <c r="CQ2" s="44"/>
+      <c r="CR2" s="44"/>
+      <c r="CS2" s="44"/>
+      <c r="CT2" s="44"/>
       <c r="CU2" s="1"/>
-      <c r="CV2" s="40" t="s">
+      <c r="CV2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="CW2" s="40"/>
-      <c r="CX2" s="40"/>
-      <c r="CY2" s="40"/>
-      <c r="CZ2" s="40"/>
-      <c r="DA2" s="40"/>
-      <c r="DB2" s="40"/>
-      <c r="DC2" s="40"/>
+      <c r="CW2" s="44"/>
+      <c r="CX2" s="44"/>
+      <c r="CY2" s="44"/>
+      <c r="CZ2" s="44"/>
+      <c r="DA2" s="44"/>
+      <c r="DB2" s="44"/>
+      <c r="DC2" s="44"/>
       <c r="DD2" s="1"/>
-      <c r="DE2" s="40" t="s">
+      <c r="DE2" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="DF2" s="40"/>
-      <c r="DG2" s="40"/>
-      <c r="DH2" s="40"/>
-      <c r="DI2" s="40"/>
-      <c r="DJ2" s="40"/>
-      <c r="DK2" s="40"/>
-      <c r="DL2" s="40"/>
+      <c r="DF2" s="44"/>
+      <c r="DG2" s="44"/>
+      <c r="DH2" s="44"/>
+      <c r="DI2" s="44"/>
+      <c r="DJ2" s="44"/>
+      <c r="DK2" s="44"/>
+      <c r="DL2" s="44"/>
       <c r="DM2" s="1"/>
-      <c r="DN2" s="40" t="s">
+      <c r="DN2" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="DO2" s="40"/>
-      <c r="DP2" s="40"/>
-      <c r="DQ2" s="40"/>
-      <c r="DR2" s="40"/>
-      <c r="DS2" s="40"/>
-      <c r="DT2" s="40"/>
-      <c r="DU2" s="40"/>
+      <c r="DO2" s="44"/>
+      <c r="DP2" s="44"/>
+      <c r="DQ2" s="44"/>
+      <c r="DR2" s="44"/>
+      <c r="DS2" s="44"/>
+      <c r="DT2" s="44"/>
+      <c r="DU2" s="44"/>
       <c r="DV2" s="1"/>
-      <c r="DW2" s="40" t="s">
+      <c r="DW2" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="DX2" s="40"/>
-      <c r="DY2" s="40"/>
-      <c r="DZ2" s="40"/>
-      <c r="EA2" s="40"/>
-      <c r="EB2" s="40"/>
-      <c r="EC2" s="40"/>
-      <c r="ED2" s="40"/>
+      <c r="DX2" s="44"/>
+      <c r="DY2" s="44"/>
+      <c r="DZ2" s="44"/>
+      <c r="EA2" s="44"/>
+      <c r="EB2" s="44"/>
+      <c r="EC2" s="44"/>
+      <c r="ED2" s="44"/>
       <c r="EE2" s="1"/>
-      <c r="EF2" s="40" t="s">
+      <c r="EF2" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="EG2" s="40"/>
-      <c r="EH2" s="40"/>
-      <c r="EI2" s="40"/>
-      <c r="EJ2" s="40"/>
-      <c r="EK2" s="40"/>
-      <c r="EL2" s="40"/>
-      <c r="EM2" s="40"/>
+      <c r="EG2" s="44"/>
+      <c r="EH2" s="44"/>
+      <c r="EI2" s="44"/>
+      <c r="EJ2" s="44"/>
+      <c r="EK2" s="44"/>
+      <c r="EL2" s="44"/>
+      <c r="EM2" s="44"/>
       <c r="EN2" s="1"/>
-      <c r="EO2" s="40" t="s">
+      <c r="EO2" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="EP2" s="40"/>
-      <c r="EQ2" s="40"/>
-      <c r="ER2" s="40"/>
-      <c r="ES2" s="40"/>
-      <c r="ET2" s="40"/>
-      <c r="EU2" s="40"/>
-      <c r="EV2" s="40"/>
+      <c r="EP2" s="44"/>
+      <c r="EQ2" s="44"/>
+      <c r="ER2" s="44"/>
+      <c r="ES2" s="44"/>
+      <c r="ET2" s="44"/>
+      <c r="EU2" s="44"/>
+      <c r="EV2" s="44"/>
       <c r="EW2" s="1"/>
-      <c r="EX2" s="40" t="s">
+      <c r="EX2" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="EY2" s="40"/>
-      <c r="EZ2" s="40"/>
-      <c r="FA2" s="40"/>
-      <c r="FB2" s="40"/>
-      <c r="FC2" s="40"/>
-      <c r="FD2" s="40"/>
-      <c r="FE2" s="40"/>
+      <c r="EY2" s="44"/>
+      <c r="EZ2" s="44"/>
+      <c r="FA2" s="44"/>
+      <c r="FB2" s="44"/>
+      <c r="FC2" s="44"/>
+      <c r="FD2" s="44"/>
+      <c r="FE2" s="44"/>
       <c r="FF2" s="1"/>
-      <c r="FG2" s="40" t="s">
+      <c r="FG2" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="FH2" s="40"/>
-      <c r="FI2" s="40"/>
-      <c r="FJ2" s="40"/>
-      <c r="FK2" s="40"/>
-      <c r="FL2" s="40"/>
-      <c r="FM2" s="40"/>
-      <c r="FN2" s="40"/>
+      <c r="FH2" s="44"/>
+      <c r="FI2" s="44"/>
+      <c r="FJ2" s="44"/>
+      <c r="FK2" s="44"/>
+      <c r="FL2" s="44"/>
+      <c r="FM2" s="44"/>
+      <c r="FN2" s="44"/>
       <c r="FO2" s="1"/>
-      <c r="FP2" s="40" t="s">
+      <c r="FP2" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="FQ2" s="40"/>
-      <c r="FR2" s="40"/>
-      <c r="FS2" s="40"/>
-      <c r="FT2" s="40"/>
-      <c r="FU2" s="40"/>
-      <c r="FV2" s="40"/>
-      <c r="FW2" s="40"/>
+      <c r="FQ2" s="44"/>
+      <c r="FR2" s="44"/>
+      <c r="FS2" s="44"/>
+      <c r="FT2" s="44"/>
+      <c r="FU2" s="44"/>
+      <c r="FV2" s="44"/>
+      <c r="FW2" s="44"/>
       <c r="FX2" s="1"/>
-      <c r="FY2" s="40" t="s">
+      <c r="FY2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="FZ2" s="40"/>
-      <c r="GA2" s="40"/>
-      <c r="GB2" s="40"/>
-      <c r="GC2" s="40"/>
-      <c r="GD2" s="40"/>
-      <c r="GE2" s="40"/>
-      <c r="GF2" s="40"/>
+      <c r="FZ2" s="44"/>
+      <c r="GA2" s="44"/>
+      <c r="GB2" s="44"/>
+      <c r="GC2" s="44"/>
+      <c r="GD2" s="44"/>
+      <c r="GE2" s="44"/>
+      <c r="GF2" s="44"/>
       <c r="GG2" s="1"/>
-      <c r="GH2" s="40" t="s">
+      <c r="GH2" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="GI2" s="40"/>
-      <c r="GJ2" s="40"/>
-      <c r="GK2" s="40"/>
-      <c r="GL2" s="40"/>
-      <c r="GM2" s="40"/>
-      <c r="GN2" s="40"/>
-      <c r="GO2" s="40"/>
+      <c r="GI2" s="44"/>
+      <c r="GJ2" s="44"/>
+      <c r="GK2" s="44"/>
+      <c r="GL2" s="44"/>
+      <c r="GM2" s="44"/>
+      <c r="GN2" s="44"/>
+      <c r="GO2" s="44"/>
       <c r="GP2" s="1"/>
     </row>
     <row r="3" spans="1:198" x14ac:dyDescent="0.2">
@@ -3710,24 +3708,24 @@
       <c r="FQ6" s="5">
         <v>2000</v>
       </c>
-      <c r="FR6" s="55">
+      <c r="FR6" s="37">
         <v>475000</v>
       </c>
-      <c r="FS6" s="55">
+      <c r="FS6" s="37">
         <f t="shared" si="19"/>
         <v>-473000</v>
       </c>
       <c r="FT6" s="5">
         <v>-10731370</v>
       </c>
-      <c r="FU6" s="55">
+      <c r="FU6" s="37">
         <v>43215800</v>
       </c>
       <c r="FV6" s="6">
         <f t="shared" si="41"/>
         <v>1.1037629755783764E-2</v>
       </c>
-      <c r="FW6" s="56">
+      <c r="FW6" s="38">
         <v>3.8100000000000002E-2</v>
       </c>
       <c r="FX6" s="1"/>
@@ -7373,7 +7371,7 @@
         <v>35708736</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D13" si="45">B13-C13</f>
         <v>-12769028</v>
       </c>
       <c r="E13" s="5">
@@ -12200,19 +12198,19 @@
       <c r="GP29" s="1"/>
     </row>
     <row r="30" spans="1:198" x14ac:dyDescent="0.2">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="36"/>
+      <c r="B30" s="39"/>
       <c r="D30" s="5">
         <f>SUM(D4:D27)</f>
         <v>-11056578</v>
       </c>
       <c r="I30" s="1"/>
-      <c r="J30" s="36" t="s">
+      <c r="J30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="K30" s="36"/>
+      <c r="K30" s="39"/>
       <c r="L30" s="5">
         <f>AVERAGE(L4:L29)</f>
         <v>887916.4</v>
@@ -12223,10 +12221,10 @@
       </c>
       <c r="N30" s="5"/>
       <c r="R30" s="1"/>
-      <c r="S30" s="36" t="s">
+      <c r="S30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="T30" s="36"/>
+      <c r="T30" s="39"/>
       <c r="U30" s="5"/>
       <c r="V30" s="5">
         <f>SUM(V3:V26)</f>
@@ -12234,10 +12232,10 @@
       </c>
       <c r="W30" s="5"/>
       <c r="AA30" s="1"/>
-      <c r="AB30" s="36" t="s">
+      <c r="AB30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="AC30" s="36"/>
+      <c r="AC30" s="39"/>
       <c r="AD30" s="5"/>
       <c r="AE30" s="5">
         <f>SUM(AE3:AE26)</f>
@@ -12245,10 +12243,10 @@
       </c>
       <c r="AF30" s="5"/>
       <c r="AJ30" s="1"/>
-      <c r="AK30" s="36" t="s">
+      <c r="AK30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="AL30" s="36"/>
+      <c r="AL30" s="39"/>
       <c r="AM30" s="5"/>
       <c r="AN30" s="5">
         <f>SUM(AN3:AN26)</f>
@@ -12256,10 +12254,10 @@
       </c>
       <c r="AO30" s="5"/>
       <c r="AS30" s="1"/>
-      <c r="AT30" s="36" t="s">
+      <c r="AT30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="AU30" s="36"/>
+      <c r="AU30" s="39"/>
       <c r="AV30" s="5"/>
       <c r="AW30" s="5">
         <f>SUM(AW3:AW26)</f>
@@ -12267,19 +12265,19 @@
       </c>
       <c r="AX30" s="5"/>
       <c r="BB30" s="1"/>
-      <c r="BC30" s="36" t="s">
+      <c r="BC30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="BD30" s="36"/>
+      <c r="BD30" s="39"/>
       <c r="BF30" s="5">
         <f>SUM(BF3:BF26)</f>
         <v>6587610</v>
       </c>
       <c r="BK30" s="1"/>
-      <c r="BL30" s="36" t="s">
+      <c r="BL30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="BM30" s="36"/>
+      <c r="BM30" s="39"/>
       <c r="BN30" s="5"/>
       <c r="BO30" s="5">
         <f>SUM(BO3:BO26)</f>
@@ -12287,10 +12285,10 @@
       </c>
       <c r="BP30" s="5"/>
       <c r="BT30" s="1"/>
-      <c r="BU30" s="36" t="s">
+      <c r="BU30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="BV30" s="36"/>
+      <c r="BV30" s="39"/>
       <c r="BW30" s="5"/>
       <c r="BX30" s="5">
         <f>SUM(BX3:BX26)</f>
@@ -12298,10 +12296,10 @@
       </c>
       <c r="BY30" s="5"/>
       <c r="CC30" s="1"/>
-      <c r="CD30" s="36" t="s">
+      <c r="CD30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="CE30" s="36"/>
+      <c r="CE30" s="39"/>
       <c r="CF30" s="5"/>
       <c r="CG30" s="5">
         <f>SUM(CG3:CG26)</f>
@@ -12309,10 +12307,10 @@
       </c>
       <c r="CH30" s="5"/>
       <c r="CL30" s="1"/>
-      <c r="CM30" s="36" t="s">
+      <c r="CM30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="CN30" s="36"/>
+      <c r="CN30" s="39"/>
       <c r="CO30" s="5"/>
       <c r="CP30" s="5">
         <f>SUM(CP3:CP26)</f>
@@ -12320,10 +12318,10 @@
       </c>
       <c r="CQ30" s="5"/>
       <c r="CU30" s="1"/>
-      <c r="CV30" s="36" t="s">
+      <c r="CV30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="CW30" s="36"/>
+      <c r="CW30" s="39"/>
       <c r="CX30" s="5"/>
       <c r="CY30" s="5">
         <f>SUM(CY3:CY26)</f>
@@ -12331,10 +12329,10 @@
       </c>
       <c r="CZ30" s="5"/>
       <c r="DD30" s="1"/>
-      <c r="DE30" s="36" t="s">
+      <c r="DE30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="DF30" s="36"/>
+      <c r="DF30" s="39"/>
       <c r="DG30" s="5"/>
       <c r="DH30" s="5">
         <f>SUM(DH3:DH26)</f>
@@ -12342,10 +12340,10 @@
       </c>
       <c r="DI30" s="5"/>
       <c r="DM30" s="1"/>
-      <c r="DN30" s="36" t="s">
+      <c r="DN30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="DO30" s="36"/>
+      <c r="DO30" s="39"/>
       <c r="DP30" s="5"/>
       <c r="DQ30" s="5">
         <f>SUM(DQ3:DQ26)</f>
@@ -12353,10 +12351,10 @@
       </c>
       <c r="DR30" s="5"/>
       <c r="DV30" s="1"/>
-      <c r="DW30" s="36" t="s">
+      <c r="DW30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="DX30" s="36"/>
+      <c r="DX30" s="39"/>
       <c r="DY30" s="5"/>
       <c r="DZ30" s="5">
         <f>SUM(DZ3:DZ26)</f>
@@ -12364,10 +12362,10 @@
       </c>
       <c r="EA30" s="5"/>
       <c r="EE30" s="1"/>
-      <c r="EF30" s="36" t="s">
+      <c r="EF30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="EG30" s="36"/>
+      <c r="EG30" s="39"/>
       <c r="EH30" s="5"/>
       <c r="EI30" s="5">
         <f>SUM(EI3:EI26)</f>
@@ -12375,10 +12373,10 @@
       </c>
       <c r="EJ30" s="5"/>
       <c r="EN30" s="1"/>
-      <c r="EO30" s="36" t="s">
+      <c r="EO30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="EP30" s="36"/>
+      <c r="EP30" s="39"/>
       <c r="EQ30" s="5"/>
       <c r="ER30" s="5">
         <f>SUM(ER3:ER26)</f>
@@ -12386,10 +12384,10 @@
       </c>
       <c r="ES30" s="5"/>
       <c r="EW30" s="1"/>
-      <c r="EX30" s="36" t="s">
+      <c r="EX30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="EY30" s="36"/>
+      <c r="EY30" s="39"/>
       <c r="EZ30" s="5"/>
       <c r="FA30" s="5">
         <f>SUM(FA3:FA26)</f>
@@ -12397,10 +12395,10 @@
       </c>
       <c r="FB30" s="5"/>
       <c r="FF30" s="1"/>
-      <c r="FG30" s="36" t="s">
+      <c r="FG30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="FH30" s="36"/>
+      <c r="FH30" s="39"/>
       <c r="FI30" s="5"/>
       <c r="FJ30" s="5">
         <f>SUM(FJ3:FJ26)</f>
@@ -12408,10 +12406,10 @@
       </c>
       <c r="FK30" s="5"/>
       <c r="FO30" s="1"/>
-      <c r="FP30" s="36" t="s">
+      <c r="FP30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="FQ30" s="36"/>
+      <c r="FQ30" s="39"/>
       <c r="FR30" s="5"/>
       <c r="FS30" s="5">
         <f>SUM(FS3:FS26)</f>
@@ -12419,10 +12417,10 @@
       </c>
       <c r="FT30" s="5"/>
       <c r="FX30" s="1"/>
-      <c r="FY30" s="36" t="s">
+      <c r="FY30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="FZ30" s="36"/>
+      <c r="FZ30" s="39"/>
       <c r="GA30" s="5"/>
       <c r="GB30" s="5">
         <f>SUM(GB3:GB26)</f>
@@ -12430,10 +12428,10 @@
       </c>
       <c r="GC30" s="5"/>
       <c r="GG30" s="1"/>
-      <c r="GH30" s="36" t="s">
+      <c r="GH30" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="GI30" s="36"/>
+      <c r="GI30" s="39"/>
       <c r="GJ30" s="5"/>
       <c r="GK30" s="5">
         <f>SUM(GK3:GK26)</f>
@@ -12443,20 +12441,20 @@
       <c r="GP30" s="1"/>
     </row>
     <row r="31" spans="1:198" x14ac:dyDescent="0.2">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="36"/>
+      <c r="B31" s="39"/>
       <c r="C31" s="5"/>
       <c r="E31" s="5">
         <f>SUM(E4:E27)</f>
         <v>134806368</v>
       </c>
       <c r="I31" s="1"/>
-      <c r="J31" s="36" t="s">
+      <c r="J31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="K31" s="36"/>
+      <c r="K31" s="39"/>
       <c r="L31" s="5"/>
       <c r="N31" s="5">
         <f>SUM(N4:N27)</f>
@@ -12464,10 +12462,10 @@
       </c>
       <c r="O31" s="5"/>
       <c r="R31" s="1"/>
-      <c r="S31" s="36" t="s">
+      <c r="S31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="T31" s="36"/>
+      <c r="T31" s="39"/>
       <c r="U31" s="5"/>
       <c r="W31" s="5">
         <f>SUM(W4:W27)</f>
@@ -12475,10 +12473,10 @@
       </c>
       <c r="X31" s="5"/>
       <c r="AA31" s="1"/>
-      <c r="AB31" s="36" t="s">
+      <c r="AB31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="AC31" s="36"/>
+      <c r="AC31" s="39"/>
       <c r="AD31" s="5"/>
       <c r="AF31" s="5">
         <f>SUM(AF4:AF27)</f>
@@ -12486,10 +12484,10 @@
       </c>
       <c r="AG31" s="5"/>
       <c r="AJ31" s="1"/>
-      <c r="AK31" s="36" t="s">
+      <c r="AK31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="AL31" s="36"/>
+      <c r="AL31" s="39"/>
       <c r="AM31" s="5"/>
       <c r="AO31" s="5">
         <f>SUM(AO4:AO27)</f>
@@ -12497,10 +12495,10 @@
       </c>
       <c r="AP31" s="5"/>
       <c r="AS31" s="1"/>
-      <c r="AT31" s="36" t="s">
+      <c r="AT31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="AU31" s="36"/>
+      <c r="AU31" s="39"/>
       <c r="AV31" s="5"/>
       <c r="AX31" s="5">
         <f>SUM(AX4:AX27)</f>
@@ -12508,19 +12506,19 @@
       </c>
       <c r="AY31" s="5"/>
       <c r="BB31" s="1"/>
-      <c r="BC31" s="36" t="s">
+      <c r="BC31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="BD31" s="36"/>
+      <c r="BD31" s="39"/>
       <c r="BG31" s="5">
         <f>SUM(BG4:BG27)</f>
         <v>147208969</v>
       </c>
       <c r="BK31" s="1"/>
-      <c r="BL31" s="36" t="s">
+      <c r="BL31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="BM31" s="36"/>
+      <c r="BM31" s="39"/>
       <c r="BN31" s="5"/>
       <c r="BP31" s="5">
         <f>SUM(BP4:BP27)</f>
@@ -12528,10 +12526,10 @@
       </c>
       <c r="BQ31" s="5"/>
       <c r="BT31" s="1"/>
-      <c r="BU31" s="36" t="s">
+      <c r="BU31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="BV31" s="36"/>
+      <c r="BV31" s="39"/>
       <c r="BW31" s="5"/>
       <c r="BY31" s="5">
         <f>SUM(BX4:BX27)</f>
@@ -12539,10 +12537,10 @@
       </c>
       <c r="BZ31" s="5"/>
       <c r="CC31" s="1"/>
-      <c r="CD31" s="36" t="s">
+      <c r="CD31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="CE31" s="36"/>
+      <c r="CE31" s="39"/>
       <c r="CF31" s="5"/>
       <c r="CH31" s="5">
         <f>SUM(CH4:CH27)</f>
@@ -12550,10 +12548,10 @@
       </c>
       <c r="CI31" s="5"/>
       <c r="CL31" s="1"/>
-      <c r="CM31" s="36" t="s">
+      <c r="CM31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="CN31" s="36"/>
+      <c r="CN31" s="39"/>
       <c r="CO31" s="5"/>
       <c r="CQ31" s="5">
         <f>SUM(CQ4:CQ27)</f>
@@ -12561,10 +12559,10 @@
       </c>
       <c r="CR31" s="5"/>
       <c r="CU31" s="1"/>
-      <c r="CV31" s="36" t="s">
+      <c r="CV31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="CW31" s="36"/>
+      <c r="CW31" s="39"/>
       <c r="CX31" s="5"/>
       <c r="CZ31" s="5">
         <f>SUM(CZ4:CZ27)</f>
@@ -12572,10 +12570,10 @@
       </c>
       <c r="DA31" s="5"/>
       <c r="DD31" s="1"/>
-      <c r="DE31" s="36" t="s">
+      <c r="DE31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="DF31" s="36"/>
+      <c r="DF31" s="39"/>
       <c r="DG31" s="5"/>
       <c r="DI31" s="5">
         <f>SUM(DI4:DI27)</f>
@@ -12583,10 +12581,10 @@
       </c>
       <c r="DJ31" s="5"/>
       <c r="DM31" s="1"/>
-      <c r="DN31" s="36" t="s">
+      <c r="DN31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="DO31" s="36"/>
+      <c r="DO31" s="39"/>
       <c r="DP31" s="5"/>
       <c r="DR31" s="5">
         <f>SUM(DR4:DR27)</f>
@@ -12594,10 +12592,10 @@
       </c>
       <c r="DS31" s="5"/>
       <c r="DV31" s="1"/>
-      <c r="DW31" s="36" t="s">
+      <c r="DW31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="DX31" s="36"/>
+      <c r="DX31" s="39"/>
       <c r="DY31" s="5"/>
       <c r="EA31" s="5">
         <f>SUM(EA4:EA27)</f>
@@ -12605,10 +12603,10 @@
       </c>
       <c r="EB31" s="5"/>
       <c r="EE31" s="1"/>
-      <c r="EF31" s="36" t="s">
+      <c r="EF31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="EG31" s="36"/>
+      <c r="EG31" s="39"/>
       <c r="EH31" s="5"/>
       <c r="EJ31" s="5">
         <f>SUM(EJ4:EJ27)</f>
@@ -12616,10 +12614,10 @@
       </c>
       <c r="EK31" s="5"/>
       <c r="EN31" s="1"/>
-      <c r="EO31" s="36" t="s">
+      <c r="EO31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="EP31" s="36"/>
+      <c r="EP31" s="39"/>
       <c r="EQ31" s="5"/>
       <c r="ES31" s="5">
         <f>SUM(ES4:ES27)</f>
@@ -12627,10 +12625,10 @@
       </c>
       <c r="ET31" s="5"/>
       <c r="EW31" s="1"/>
-      <c r="EX31" s="36" t="s">
+      <c r="EX31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="EY31" s="36"/>
+      <c r="EY31" s="39"/>
       <c r="EZ31" s="5"/>
       <c r="FB31" s="5">
         <f>SUM(FB4:FB27)</f>
@@ -12638,10 +12636,10 @@
       </c>
       <c r="FC31" s="5"/>
       <c r="FF31" s="1"/>
-      <c r="FG31" s="36" t="s">
+      <c r="FG31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="FH31" s="36"/>
+      <c r="FH31" s="39"/>
       <c r="FI31" s="5"/>
       <c r="FK31" s="5">
         <f>SUM(FK4:FK27)</f>
@@ -12649,10 +12647,10 @@
       </c>
       <c r="FL31" s="5"/>
       <c r="FO31" s="1"/>
-      <c r="FP31" s="36" t="s">
+      <c r="FP31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="FQ31" s="36"/>
+      <c r="FQ31" s="39"/>
       <c r="FR31" s="5"/>
       <c r="FT31" s="5">
         <f>SUM(FT4:FT27)</f>
@@ -12660,10 +12658,10 @@
       </c>
       <c r="FU31" s="5"/>
       <c r="FX31" s="1"/>
-      <c r="FY31" s="36" t="s">
+      <c r="FY31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="FZ31" s="36"/>
+      <c r="FZ31" s="39"/>
       <c r="GA31" s="5"/>
       <c r="GC31" s="5">
         <f>SUM(GC4:GC27)</f>
@@ -12671,10 +12669,10 @@
       </c>
       <c r="GD31" s="5"/>
       <c r="GG31" s="1"/>
-      <c r="GH31" s="36" t="s">
+      <c r="GH31" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="GI31" s="36"/>
+      <c r="GI31" s="39"/>
       <c r="GJ31" s="5"/>
       <c r="GL31" s="5">
         <f>SUM(GL4:GL27)</f>
@@ -12684,220 +12682,220 @@
       <c r="GP31" s="1"/>
     </row>
     <row r="32" spans="1:198" x14ac:dyDescent="0.2">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="36"/>
+      <c r="B32" s="39"/>
       <c r="F32" s="5"/>
       <c r="H32" s="9">
         <f>SUM(H4:H27)</f>
         <v>4.2499999999999996E-2</v>
       </c>
       <c r="I32" s="1"/>
-      <c r="J32" s="36" t="s">
+      <c r="J32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="K32" s="36"/>
+      <c r="K32" s="39"/>
       <c r="O32" s="5"/>
       <c r="Q32" s="9">
         <f>SUM(Q4:Q27)</f>
         <v>1.9699999999999995E-2</v>
       </c>
       <c r="R32" s="1"/>
-      <c r="S32" s="36" t="s">
+      <c r="S32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="T32" s="36"/>
+      <c r="T32" s="39"/>
       <c r="X32" s="5"/>
       <c r="Z32" s="9">
         <f>SUM(Z4:Z27)</f>
         <v>-6.9000000000000034E-3</v>
       </c>
       <c r="AA32" s="1"/>
-      <c r="AB32" s="36" t="s">
+      <c r="AB32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="AC32" s="36"/>
+      <c r="AC32" s="39"/>
       <c r="AG32" s="5"/>
       <c r="AI32" s="9">
         <f>SUM(AI4:AI27)</f>
         <v>5.9999999999999984E-4</v>
       </c>
       <c r="AJ32" s="1"/>
-      <c r="AK32" s="36" t="s">
+      <c r="AK32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="AL32" s="36"/>
+      <c r="AL32" s="39"/>
       <c r="AP32" s="5"/>
       <c r="AR32" s="9">
         <f>SUM(AR4:AR27)</f>
         <v>-2.4199999999999999E-2</v>
       </c>
       <c r="AS32" s="1"/>
-      <c r="AT32" s="36" t="s">
+      <c r="AT32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="AU32" s="36"/>
+      <c r="AU32" s="39"/>
       <c r="AY32" s="5"/>
       <c r="BA32" s="9">
         <f>SUM(BA4:BA27)</f>
         <v>2.4800000000000006E-2</v>
       </c>
       <c r="BB32" s="1"/>
-      <c r="BC32" s="36" t="s">
+      <c r="BC32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="BD32" s="36"/>
+      <c r="BD32" s="39"/>
       <c r="BH32" s="5"/>
       <c r="BJ32" s="9">
         <f>SUM(BJ4:BJ27)</f>
         <v>7.5500000000000012E-2</v>
       </c>
       <c r="BK32" s="1"/>
-      <c r="BL32" s="36" t="s">
+      <c r="BL32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="BM32" s="36"/>
+      <c r="BM32" s="39"/>
       <c r="BQ32" s="5"/>
       <c r="BS32" s="9">
         <f>SUM(BS4:BS27)</f>
         <v>-6.25E-2</v>
       </c>
       <c r="BT32" s="1"/>
-      <c r="BU32" s="36" t="s">
+      <c r="BU32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="BV32" s="36"/>
+      <c r="BV32" s="39"/>
       <c r="BZ32" s="5"/>
       <c r="CB32" s="9">
         <f>SUM(CB4:CB27)</f>
         <v>3.8000000000000048E-3</v>
       </c>
       <c r="CC32" s="1"/>
-      <c r="CD32" s="36" t="s">
+      <c r="CD32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="CE32" s="36"/>
+      <c r="CE32" s="39"/>
       <c r="CI32" s="5"/>
       <c r="CK32" s="9">
         <f>SUM(CK4:CK27)</f>
         <v>2.3999999999999976E-3</v>
       </c>
       <c r="CL32" s="1"/>
-      <c r="CM32" s="36" t="s">
+      <c r="CM32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="CN32" s="36"/>
+      <c r="CN32" s="39"/>
       <c r="CR32" s="5"/>
       <c r="CT32" s="9">
         <f>SUM(CT4:CT27)</f>
         <v>6.88E-2</v>
       </c>
       <c r="CU32" s="1"/>
-      <c r="CV32" s="36" t="s">
+      <c r="CV32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="CW32" s="36"/>
+      <c r="CW32" s="39"/>
       <c r="DA32" s="5"/>
       <c r="DC32" s="9">
         <f>SUM(DC4:DC27)</f>
         <v>5.5499999999999987E-2</v>
       </c>
       <c r="DD32" s="1"/>
-      <c r="DE32" s="36" t="s">
+      <c r="DE32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="DF32" s="36"/>
+      <c r="DF32" s="39"/>
       <c r="DJ32" s="5"/>
       <c r="DL32" s="9">
         <f>SUM(DL4:DL27)</f>
         <v>1.1799999999999995E-2</v>
       </c>
       <c r="DM32" s="1"/>
-      <c r="DN32" s="36" t="s">
+      <c r="DN32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="DO32" s="36"/>
+      <c r="DO32" s="39"/>
       <c r="DS32" s="5"/>
       <c r="DU32" s="9">
         <f>SUM(DU4:DU27)</f>
         <v>0.11399999999999999</v>
       </c>
       <c r="DV32" s="1"/>
-      <c r="DW32" s="36" t="s">
+      <c r="DW32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="DX32" s="36"/>
+      <c r="DX32" s="39"/>
       <c r="EB32" s="5"/>
       <c r="ED32" s="9">
         <f>SUM(ED4:ED27)</f>
         <v>1.7300000000000003E-2</v>
       </c>
       <c r="EE32" s="1"/>
-      <c r="EF32" s="36" t="s">
+      <c r="EF32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="EG32" s="36"/>
+      <c r="EG32" s="39"/>
       <c r="EK32" s="5"/>
       <c r="EM32" s="9">
         <f>SUM(EM4:EM27)</f>
         <v>3.6699999999999997E-2</v>
       </c>
       <c r="EN32" s="1"/>
-      <c r="EO32" s="36" t="s">
+      <c r="EO32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="EP32" s="36"/>
+      <c r="EP32" s="39"/>
       <c r="ET32" s="5"/>
       <c r="EV32" s="9">
         <f>SUM(EV4:EV27)</f>
         <v>7.51E-2</v>
       </c>
       <c r="EW32" s="1"/>
-      <c r="EX32" s="36" t="s">
+      <c r="EX32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="EY32" s="36"/>
+      <c r="EY32" s="39"/>
       <c r="FC32" s="5"/>
       <c r="FE32" s="9">
         <f>SUM(FE4:FE27)</f>
         <v>7.2499999999999995E-2</v>
       </c>
       <c r="FF32" s="1"/>
-      <c r="FG32" s="36" t="s">
+      <c r="FG32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="FH32" s="36"/>
+      <c r="FH32" s="39"/>
       <c r="FL32" s="5"/>
       <c r="FN32" s="9">
         <f>SUM(FN4:FN27)</f>
         <v>-1.4099999999999991E-2</v>
       </c>
       <c r="FO32" s="1"/>
-      <c r="FP32" s="36" t="s">
+      <c r="FP32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="FQ32" s="36"/>
+      <c r="FQ32" s="39"/>
       <c r="FU32" s="5"/>
       <c r="FW32" s="9">
         <f>SUM(FW4:FW27)</f>
         <v>4.4300000000000006E-2</v>
       </c>
       <c r="FX32" s="1"/>
-      <c r="FY32" s="36" t="s">
+      <c r="FY32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="FZ32" s="36"/>
+      <c r="FZ32" s="39"/>
       <c r="GD32" s="5"/>
       <c r="GF32" s="9">
         <f>SUM(GF4:GF27)</f>
         <v>3.5200000000000009E-2</v>
       </c>
       <c r="GG32" s="1"/>
-      <c r="GH32" s="36" t="s">
+      <c r="GH32" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="GI32" s="36"/>
+      <c r="GI32" s="39"/>
       <c r="GM32" s="5"/>
       <c r="GO32" s="9">
         <f>SUM(GO4:GO27)</f>
@@ -12906,199 +12904,199 @@
       <c r="GP32" s="1"/>
     </row>
     <row r="33" spans="1:198" x14ac:dyDescent="0.2">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="36"/>
+      <c r="B33" s="39"/>
       <c r="H33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="36" t="s">
+      <c r="J33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="K33" s="36"/>
+      <c r="K33" s="39"/>
       <c r="Q33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="R33" s="1"/>
-      <c r="S33" s="36" t="s">
+      <c r="S33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="T33" s="36"/>
+      <c r="T33" s="39"/>
       <c r="Z33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="AA33" s="1"/>
-      <c r="AB33" s="36" t="s">
+      <c r="AB33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="AC33" s="36"/>
+      <c r="AC33" s="39"/>
       <c r="AI33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="AJ33" s="1"/>
-      <c r="AK33" s="36" t="s">
+      <c r="AK33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="AL33" s="36"/>
+      <c r="AL33" s="39"/>
       <c r="AR33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="AS33" s="1"/>
-      <c r="AT33" s="36" t="s">
+      <c r="AT33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="AU33" s="36"/>
+      <c r="AU33" s="39"/>
       <c r="BA33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="BB33" s="1"/>
-      <c r="BC33" s="36" t="s">
+      <c r="BC33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="BD33" s="36"/>
+      <c r="BD33" s="39"/>
       <c r="BJ33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="BK33" s="1"/>
-      <c r="BL33" s="36" t="s">
+      <c r="BL33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="BM33" s="36"/>
+      <c r="BM33" s="39"/>
       <c r="BS33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="BT33" s="1"/>
-      <c r="BU33" s="36" t="s">
+      <c r="BU33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="BV33" s="36"/>
+      <c r="BV33" s="39"/>
       <c r="CB33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="CC33" s="1"/>
-      <c r="CD33" s="36" t="s">
+      <c r="CD33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="CE33" s="36"/>
+      <c r="CE33" s="39"/>
       <c r="CK33" s="9">
         <f>'VNINDEX T11-T12'!M36</f>
         <v>0</v>
       </c>
       <c r="CL33" s="1"/>
-      <c r="CM33" s="36" t="s">
+      <c r="CM33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="CN33" s="36"/>
+      <c r="CN33" s="39"/>
       <c r="CT33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="CU33" s="1"/>
-      <c r="CV33" s="36" t="s">
+      <c r="CV33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="CW33" s="36"/>
+      <c r="CW33" s="39"/>
       <c r="DC33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="DD33" s="1"/>
-      <c r="DE33" s="36" t="s">
+      <c r="DE33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="DF33" s="36"/>
+      <c r="DF33" s="39"/>
       <c r="DL33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="DM33" s="1"/>
-      <c r="DN33" s="36" t="s">
+      <c r="DN33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="DO33" s="36"/>
+      <c r="DO33" s="39"/>
       <c r="DU33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="DV33" s="1"/>
-      <c r="DW33" s="36" t="s">
+      <c r="DW33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="DX33" s="36"/>
+      <c r="DX33" s="39"/>
       <c r="ED33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="EE33" s="1"/>
-      <c r="EF33" s="36" t="s">
+      <c r="EF33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="EG33" s="36"/>
+      <c r="EG33" s="39"/>
       <c r="EM33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="EN33" s="1"/>
-      <c r="EO33" s="36" t="s">
+      <c r="EO33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="EP33" s="36"/>
+      <c r="EP33" s="39"/>
       <c r="EV33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="EW33" s="1"/>
-      <c r="EX33" s="36" t="s">
+      <c r="EX33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="EY33" s="36"/>
+      <c r="EY33" s="39"/>
       <c r="FE33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="FF33" s="1"/>
-      <c r="FG33" s="36" t="s">
+      <c r="FG33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="FH33" s="36"/>
+      <c r="FH33" s="39"/>
       <c r="FN33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="FO33" s="1"/>
-      <c r="FP33" s="36" t="s">
+      <c r="FP33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="FQ33" s="36"/>
+      <c r="FQ33" s="39"/>
       <c r="FW33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="FX33" s="1"/>
-      <c r="FY33" s="36" t="s">
+      <c r="FY33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="FZ33" s="36"/>
+      <c r="FZ33" s="39"/>
       <c r="GF33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
       </c>
       <c r="GG33" s="1"/>
-      <c r="GH33" s="36" t="s">
+      <c r="GH33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="GI33" s="36"/>
+      <c r="GI33" s="39"/>
       <c r="GO33" s="9">
         <f>'VNINDEX T11-T12'!D36</f>
         <v>1.1999999999999971E-3</v>
@@ -13121,35 +13119,64 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="120">
-    <mergeCell ref="CD31:CE31"/>
-    <mergeCell ref="CD32:CE32"/>
-    <mergeCell ref="CD33:CE33"/>
-    <mergeCell ref="BK1:CK1"/>
-    <mergeCell ref="S1:AR1"/>
-    <mergeCell ref="DN32:DO32"/>
-    <mergeCell ref="DW32:DX32"/>
-    <mergeCell ref="FG32:FH32"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="EF32:EG32"/>
-    <mergeCell ref="EO32:EP32"/>
-    <mergeCell ref="EX32:EY32"/>
-    <mergeCell ref="FP32:FQ32"/>
-    <mergeCell ref="BC31:BD31"/>
-    <mergeCell ref="BL31:BM31"/>
-    <mergeCell ref="BU31:BV31"/>
-    <mergeCell ref="CM31:CN31"/>
-    <mergeCell ref="CV31:CW31"/>
-    <mergeCell ref="DE31:DF31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="AB31:AC31"/>
-    <mergeCell ref="AK31:AL31"/>
-    <mergeCell ref="AT31:AU31"/>
-    <mergeCell ref="EF30:EG30"/>
-    <mergeCell ref="EO30:EP30"/>
-    <mergeCell ref="EX30:EY30"/>
+  <mergeCells count="119">
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="AB33:AC33"/>
+    <mergeCell ref="AK33:AL33"/>
+    <mergeCell ref="FY33:FZ33"/>
+    <mergeCell ref="GH33:GI33"/>
+    <mergeCell ref="EF33:EG33"/>
+    <mergeCell ref="EO33:EP33"/>
+    <mergeCell ref="EX33:EY33"/>
+    <mergeCell ref="FG33:FH33"/>
+    <mergeCell ref="FP33:FQ33"/>
+    <mergeCell ref="CM33:CN33"/>
+    <mergeCell ref="CV33:CW33"/>
+    <mergeCell ref="DE33:DF33"/>
+    <mergeCell ref="DN33:DO33"/>
+    <mergeCell ref="DW33:DX33"/>
+    <mergeCell ref="AT30:AU30"/>
+    <mergeCell ref="BC30:BD30"/>
+    <mergeCell ref="BL30:BM30"/>
+    <mergeCell ref="CD2:CK2"/>
+    <mergeCell ref="CD30:CE30"/>
+    <mergeCell ref="AT33:AU33"/>
+    <mergeCell ref="BC33:BD33"/>
+    <mergeCell ref="BL33:BM33"/>
+    <mergeCell ref="BU33:BV33"/>
+    <mergeCell ref="BC2:BJ2"/>
+    <mergeCell ref="BL2:BR2"/>
+    <mergeCell ref="BU2:CB2"/>
+    <mergeCell ref="CM2:CT2"/>
+    <mergeCell ref="CV2:DC2"/>
+    <mergeCell ref="DE2:DL2"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="S2:Z2"/>
+    <mergeCell ref="AB2:AI2"/>
+    <mergeCell ref="GH1:GO1"/>
+    <mergeCell ref="FY1:GF1"/>
+    <mergeCell ref="FP1:FW1"/>
+    <mergeCell ref="FG2:FN2"/>
+    <mergeCell ref="FG30:FH30"/>
+    <mergeCell ref="FG31:FH31"/>
+    <mergeCell ref="EW1:FN1"/>
+    <mergeCell ref="FY31:FZ31"/>
+    <mergeCell ref="FY30:FZ30"/>
+    <mergeCell ref="GH30:GI30"/>
+    <mergeCell ref="CM30:CN30"/>
+    <mergeCell ref="CV30:CW30"/>
+    <mergeCell ref="DE30:DF30"/>
+    <mergeCell ref="DN30:DO30"/>
+    <mergeCell ref="DW30:DX30"/>
+    <mergeCell ref="FY2:GF2"/>
+    <mergeCell ref="GH2:GO2"/>
+    <mergeCell ref="EF2:EM2"/>
+    <mergeCell ref="EO2:EV2"/>
+    <mergeCell ref="EX2:FE2"/>
+    <mergeCell ref="DN2:DU2"/>
+    <mergeCell ref="DW2:ED2"/>
     <mergeCell ref="FP30:FQ30"/>
     <mergeCell ref="FP2:FW2"/>
     <mergeCell ref="AK2:AR2"/>
@@ -13174,74 +13201,44 @@
     <mergeCell ref="BU32:BV32"/>
     <mergeCell ref="CM32:CN32"/>
     <mergeCell ref="CV32:CW32"/>
+    <mergeCell ref="FP32:FQ32"/>
+    <mergeCell ref="BC31:BD31"/>
+    <mergeCell ref="BL31:BM31"/>
+    <mergeCell ref="BU31:BV31"/>
+    <mergeCell ref="CM31:CN31"/>
+    <mergeCell ref="CV31:CW31"/>
+    <mergeCell ref="DE31:DF31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="S31:T31"/>
+    <mergeCell ref="AB31:AC31"/>
+    <mergeCell ref="AK31:AL31"/>
+    <mergeCell ref="AT31:AU31"/>
     <mergeCell ref="DE32:DF32"/>
+    <mergeCell ref="CD31:CE31"/>
+    <mergeCell ref="CD32:CE32"/>
+    <mergeCell ref="CD33:CE33"/>
+    <mergeCell ref="BK1:CK1"/>
+    <mergeCell ref="S1:AR1"/>
+    <mergeCell ref="DN32:DO32"/>
+    <mergeCell ref="DW32:DX32"/>
+    <mergeCell ref="FG32:FH32"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="EF32:EG32"/>
+    <mergeCell ref="EO32:EP32"/>
+    <mergeCell ref="EX32:EY32"/>
+    <mergeCell ref="EF30:EG30"/>
+    <mergeCell ref="EO30:EP30"/>
+    <mergeCell ref="EX30:EY30"/>
     <mergeCell ref="EE1:EU1"/>
-    <mergeCell ref="GH1:GO1"/>
-    <mergeCell ref="FY1:GF1"/>
-    <mergeCell ref="FP1:FW1"/>
-    <mergeCell ref="CL1:EC1"/>
-    <mergeCell ref="FG2:FN2"/>
-    <mergeCell ref="FG30:FH30"/>
-    <mergeCell ref="FG31:FH31"/>
-    <mergeCell ref="EW1:FN1"/>
-    <mergeCell ref="FY31:FZ31"/>
-    <mergeCell ref="FY30:FZ30"/>
-    <mergeCell ref="GH30:GI30"/>
     <mergeCell ref="BU30:BV30"/>
-    <mergeCell ref="CM30:CN30"/>
-    <mergeCell ref="CV30:CW30"/>
-    <mergeCell ref="DE30:DF30"/>
-    <mergeCell ref="DN30:DO30"/>
-    <mergeCell ref="DW30:DX30"/>
-    <mergeCell ref="FY2:GF2"/>
-    <mergeCell ref="GH2:GO2"/>
-    <mergeCell ref="EF2:EM2"/>
-    <mergeCell ref="EO2:EV2"/>
-    <mergeCell ref="EX2:FE2"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="AS1:BI1"/>
-    <mergeCell ref="DN2:DU2"/>
-    <mergeCell ref="DW2:ED2"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="S30:T30"/>
     <mergeCell ref="AB30:AC30"/>
     <mergeCell ref="AK30:AL30"/>
-    <mergeCell ref="BC2:BJ2"/>
-    <mergeCell ref="BL2:BR2"/>
-    <mergeCell ref="BU2:CB2"/>
-    <mergeCell ref="CM2:CT2"/>
-    <mergeCell ref="CV2:DC2"/>
-    <mergeCell ref="DE2:DL2"/>
-    <mergeCell ref="J2:Q2"/>
-    <mergeCell ref="S2:Z2"/>
-    <mergeCell ref="AB2:AI2"/>
-    <mergeCell ref="AT30:AU30"/>
-    <mergeCell ref="BC30:BD30"/>
-    <mergeCell ref="BL30:BM30"/>
-    <mergeCell ref="CD2:CK2"/>
-    <mergeCell ref="CD30:CE30"/>
-    <mergeCell ref="AT33:AU33"/>
-    <mergeCell ref="BC33:BD33"/>
-    <mergeCell ref="BL33:BM33"/>
-    <mergeCell ref="BU33:BV33"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="AB33:AC33"/>
-    <mergeCell ref="AK33:AL33"/>
-    <mergeCell ref="FY33:FZ33"/>
-    <mergeCell ref="GH33:GI33"/>
-    <mergeCell ref="EF33:EG33"/>
-    <mergeCell ref="EO33:EP33"/>
-    <mergeCell ref="EX33:EY33"/>
-    <mergeCell ref="FG33:FH33"/>
-    <mergeCell ref="FP33:FQ33"/>
-    <mergeCell ref="CM33:CN33"/>
-    <mergeCell ref="CV33:CW33"/>
-    <mergeCell ref="DE33:DF33"/>
-    <mergeCell ref="DN33:DO33"/>
-    <mergeCell ref="DW33:DX33"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F7">
     <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
@@ -13267,19 +13264,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -14125,11 +14122,11 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="54">
+      <c r="B36" s="39"/>
+      <c r="C36" s="36">
         <f>SUM(C3:C34)</f>
         <v>0.97000000000000064</v>
       </c>
@@ -14139,20 +14136,20 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="36"/>
+      <c r="B37" s="39"/>
       <c r="F37" s="5">
         <f>AVERAGE(F3:F34)</f>
         <v>770590152.79999995</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="36"/>
+      <c r="B38" s="39"/>
       <c r="E38" s="9">
         <f>AVERAGE(E3:E34)</f>
         <v>1.4749999999999999E-2</v>

</xml_diff>